<commit_message>
agrego cotas y corrijo rnf
</commit_message>
<xml_diff>
--- a/Documentacion/Entrega 0/Tabla de Decisiones.xlsx
+++ b/Documentacion/Entrega 0/Tabla de Decisiones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martìn\Desktop\TP SISTEMAS\G6_S_G_E\Documentacion\Entrega 0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{750F47C5-F10F-46B5-B3E6-633C8FE40FC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76F4F5F-C093-4F68-AEBB-D0BB3C83CEED}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Alternativa</t>
   </si>
   <si>
-    <t>Java</t>
-  </si>
-  <si>
     <t>Al no ser puro OO algunas veces trae dolores de cabeza</t>
   </si>
   <si>
@@ -153,11 +150,14 @@
   <si>
     <t>Generar métodos correspondientes en cada clase</t>
   </si>
+  <si>
+    <t>Lenguaje de programacion Java</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,11 +601,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,33 +638,33 @@
         <v>43187</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>43204</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -672,16 +672,16 @@
         <v>43204</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -689,16 +689,16 @@
         <v>43208</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -706,16 +706,16 @@
         <v>43208</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -723,16 +723,16 @@
         <v>43214</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -740,33 +740,33 @@
         <v>43208</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>